<commit_message>
updated xls sheet labels
</commit_message>
<xml_diff>
--- a/data/scenarios.xlsx
+++ b/data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneriddell/Documents/repos/Guide-to-DID-estimators/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C8933B-F90F-F241-94CF-4572D9AFE903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F973FD3C-53A3-364D-A11D-EE63A87A1899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45480" yWindow="1400" windowWidth="26860" windowHeight="18780" activeTab="8" xr2:uid="{3A84A3DE-CD8F-5C4B-BB69-5AB88BC02DD1}"/>
+    <workbookView xWindow="-45480" yWindow="1400" windowWidth="26860" windowHeight="18780" activeTab="10" xr2:uid="{3A84A3DE-CD8F-5C4B-BB69-5AB88BC02DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="scen1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="scen4" sheetId="6" r:id="rId6"/>
     <sheet name="scen5" sheetId="7" r:id="rId7"/>
     <sheet name="scen6" sheetId="9" r:id="rId8"/>
-    <sheet name="scen9" sheetId="13" r:id="rId9"/>
-    <sheet name="scen7" sheetId="10" r:id="rId10"/>
-    <sheet name="scen8" sheetId="12" r:id="rId11"/>
+    <sheet name="scen7" sheetId="13" r:id="rId9"/>
+    <sheet name="scen8" sheetId="10" r:id="rId10"/>
+    <sheet name="scen9" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32EF42-1665-1742-8ED8-18BCC709F02B}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3169,7 +3169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614FFDD6-16D5-BA47-8A1C-7C7CB4FDA225}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -12553,10 +12553,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8D1594-9425-564C-987A-9BFC085D0B14}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13782,7 +13782,7 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <f>D46+3</f>
+        <f t="shared" ref="D47:D61" si="2">D46+3</f>
         <v>33</v>
       </c>
       <c r="E47">
@@ -13802,7 +13802,7 @@
         <v>27</v>
       </c>
       <c r="J47" s="7">
-        <f t="shared" ref="J47:J60" si="2">D47-I47</f>
+        <f t="shared" ref="J47:J60" si="3">D47-I47</f>
         <v>6</v>
       </c>
     </row>
@@ -13817,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <f>D47+3</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="E48">
@@ -13833,11 +13833,11 @@
         <v>42125</v>
       </c>
       <c r="I48" s="7">
-        <f t="shared" ref="I48:I61" si="3">I47+3</f>
+        <f t="shared" ref="I48:I61" si="4">I47+3</f>
         <v>30</v>
       </c>
       <c r="J48" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
@@ -13852,7 +13852,7 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <f>D48+3</f>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="E49">
@@ -13868,11 +13868,11 @@
         <v>42125</v>
       </c>
       <c r="I49" s="7">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="J49" s="7">
         <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="J49" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -13887,7 +13887,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <f>D49+3</f>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="E50">
@@ -13903,11 +13903,11 @@
         <v>42125</v>
       </c>
       <c r="I50" s="7">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="J50" s="7">
         <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="J50" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -13922,7 +13922,7 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <f>D50+3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="E51">
@@ -13938,11 +13938,11 @@
         <v>42125</v>
       </c>
       <c r="I51" s="7">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="J51" s="7">
         <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="J51" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -13957,7 +13957,7 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <f>D51+3</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="E52">
@@ -13973,11 +13973,11 @@
         <v>42125</v>
       </c>
       <c r="I52" s="7">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="J52" s="7">
         <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="J52" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -13992,7 +13992,7 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <f>D52+3</f>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="E53">
@@ -14008,11 +14008,11 @@
         <v>42125</v>
       </c>
       <c r="I53" s="7">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="J53" s="7">
         <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="J53" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14027,7 +14027,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <f>D53+3</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="E54">
@@ -14043,11 +14043,11 @@
         <v>42125</v>
       </c>
       <c r="I54" s="7">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="J54" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="J54" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14062,7 +14062,7 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <f>D54+3</f>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="E55">
@@ -14078,11 +14078,11 @@
         <v>42125</v>
       </c>
       <c r="I55" s="7">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="J55" s="7">
         <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="J55" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14097,7 +14097,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <f>D55+3</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="E56">
@@ -14113,11 +14113,11 @@
         <v>42125</v>
       </c>
       <c r="I56" s="7">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="J56" s="7">
         <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-      <c r="J56" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14132,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <f>D56+3</f>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="E57">
@@ -14148,11 +14148,11 @@
         <v>42125</v>
       </c>
       <c r="I57" s="7">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="J57" s="7">
         <f t="shared" si="3"/>
-        <v>57</v>
-      </c>
-      <c r="J57" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14167,7 +14167,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <f>D57+3</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="E58">
@@ -14183,11 +14183,11 @@
         <v>42125</v>
       </c>
       <c r="I58" s="7">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="J58" s="7">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="J58" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14202,7 +14202,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <f>D58+3</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="E59">
@@ -14218,11 +14218,11 @@
         <v>42125</v>
       </c>
       <c r="I59" s="7">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="J59" s="7">
         <f t="shared" si="3"/>
-        <v>63</v>
-      </c>
-      <c r="J59" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14237,7 +14237,7 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <f>D59+3</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="E60">
@@ -14253,11 +14253,11 @@
         <v>42125</v>
       </c>
       <c r="I60" s="7">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="J60" s="7">
         <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="J60" s="7">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -14272,7 +14272,7 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <f>D60+3</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="E61">
@@ -14288,7 +14288,7 @@
         <v>42125</v>
       </c>
       <c r="I61" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="J61" s="7">
@@ -14336,7 +14336,7 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <f t="shared" ref="D63:D72" si="4">D23+8</f>
+        <f t="shared" ref="D63:D72" si="5">D23+8</f>
         <v>21</v>
       </c>
       <c r="E63">
@@ -14365,7 +14365,7 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="E64">
@@ -14383,7 +14383,7 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4</v>
       </c>
@@ -14394,7 +14394,7 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="E65">
@@ -14412,7 +14412,7 @@
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>4</v>
       </c>
@@ -14423,7 +14423,7 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E66">
@@ -14441,7 +14441,7 @@
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>4</v>
       </c>
@@ -14452,7 +14452,7 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="E67">
@@ -14470,7 +14470,7 @@
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>4</v>
       </c>
@@ -14481,7 +14481,7 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="E68">
@@ -14499,7 +14499,7 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>4</v>
       </c>
@@ -14510,7 +14510,7 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="E69">
@@ -14528,7 +14528,7 @@
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>4</v>
       </c>
@@ -14539,7 +14539,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="E70">
@@ -14557,7 +14557,7 @@
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>4</v>
       </c>
@@ -14568,7 +14568,7 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="E71">
@@ -14586,7 +14586,7 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>4</v>
       </c>
@@ -14597,7 +14597,7 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="E72">
@@ -14615,7 +14615,7 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>4</v>
       </c>
@@ -14626,7 +14626,7 @@
         <v>1</v>
       </c>
       <c r="D73">
-        <f>D33+12</f>
+        <f t="shared" ref="D73:D81" si="6">D33+12</f>
         <v>55</v>
       </c>
       <c r="E73">
@@ -14649,8 +14649,16 @@
         <f>D73-I73</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L73">
+        <f>(2*5*9 + 1*6*7)/25</f>
+        <v>5.28</v>
+      </c>
+      <c r="M73">
+        <f>(5*9 + 6*7)/16</f>
+        <v>5.4375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4</v>
       </c>
@@ -14661,7 +14669,7 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <f>D34+12</f>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="E74">
@@ -14681,11 +14689,11 @@
         <v>54</v>
       </c>
       <c r="J74" s="7">
-        <f t="shared" ref="J74:J81" si="5">D74-I74</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" ref="J74:J81" si="7">D74-I74</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
@@ -14696,7 +14704,7 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <f>D35+12</f>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="E75">
@@ -14712,15 +14720,15 @@
         <v>42339</v>
       </c>
       <c r="I75" s="7">
-        <f t="shared" ref="I75:I81" si="6">I74+3</f>
+        <f t="shared" ref="I75:I81" si="8">I74+3</f>
         <v>57</v>
       </c>
       <c r="J75" s="7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4</v>
       </c>
@@ -14731,7 +14739,7 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <f>D36+12</f>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="E76">
@@ -14747,15 +14755,15 @@
         <v>42339</v>
       </c>
       <c r="I76" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="J76" s="7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4</v>
       </c>
@@ -14766,7 +14774,7 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <f>D37+12</f>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="E77">
@@ -14782,15 +14790,15 @@
         <v>42339</v>
       </c>
       <c r="I77" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="J77" s="7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>4</v>
       </c>
@@ -14801,7 +14809,7 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <f>D38+12</f>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="E78">
@@ -14817,15 +14825,15 @@
         <v>42339</v>
       </c>
       <c r="I78" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>66</v>
       </c>
       <c r="J78" s="7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>4</v>
       </c>
@@ -14836,7 +14844,7 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <f>D39+12</f>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="E79">
@@ -14852,15 +14860,15 @@
         <v>42339</v>
       </c>
       <c r="I79" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>69</v>
       </c>
       <c r="J79" s="7">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>4</v>
       </c>
@@ -14871,7 +14879,7 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <f>D40+12</f>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="E80">
@@ -14887,11 +14895,11 @@
         <v>42339</v>
       </c>
       <c r="I80" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>72</v>
       </c>
       <c r="J80" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
@@ -14906,7 +14914,7 @@
         <v>1</v>
       </c>
       <c r="D81">
-        <f>D41+12</f>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="E81">
@@ -14922,11 +14930,11 @@
         <v>42339</v>
       </c>
       <c r="I81" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
       <c r="J81" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>

</xml_diff>